<commit_message>
New test using dlookr
Wanted to test and see the automatic report feature from dlookr
</commit_message>
<xml_diff>
--- a/Development/datasets/Utrecht2019dataset.xlsx
+++ b/Development/datasets/Utrecht2019dataset.xlsx
@@ -1510,8 +1510,8 @@
   </sheetPr>
   <dimension ref="A1:I648"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A613" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B637" activeCellId="0" sqref="B637"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5075,9 +5075,6 @@
       <c r="B156" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C156" s="1" t="n">
-        <v>9990</v>
-      </c>
       <c r="D156" s="1" t="n">
         <v>0</v>
       </c>
@@ -7311,9 +7308,6 @@
       <c r="A254" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B254" s="1" t="n">
-        <v>999</v>
-      </c>
       <c r="C254" s="1" t="n">
         <v>0</v>
       </c>
@@ -7403,9 +7397,6 @@
       <c r="A258" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B258" s="1" t="n">
-        <v>999</v>
-      </c>
       <c r="C258" s="1" t="n">
         <v>0</v>
       </c>
@@ -10484,9 +10475,6 @@
       <c r="A393" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B393" s="1" t="n">
-        <v>999</v>
-      </c>
       <c r="C393" s="1" t="n">
         <v>0</v>
       </c>
@@ -10849,9 +10837,6 @@
       <c r="B409" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C409" s="1" t="n">
-        <v>9990</v>
-      </c>
       <c r="D409" s="1" t="n">
         <v>1</v>
       </c>
@@ -11697,9 +11682,6 @@
       <c r="B446" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C446" s="1" t="n">
-        <v>9990</v>
-      </c>
       <c r="D446" s="1" t="n">
         <v>1</v>
       </c>
@@ -12111,9 +12093,6 @@
       <c r="B464" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C464" s="1" t="n">
-        <v>9990</v>
-      </c>
       <c r="D464" s="1" t="n">
         <v>1</v>
       </c>
@@ -12614,9 +12593,6 @@
       <c r="B486" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C486" s="1" t="n">
-        <v>9990</v>
-      </c>
       <c r="D486" s="1" t="n">
         <v>1</v>
       </c>
@@ -16053,9 +16029,6 @@
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="1" t="n">
         <v>68</v>
-      </c>
-      <c r="B637" s="1" t="n">
-        <v>999</v>
       </c>
       <c r="C637" s="1" t="n">
         <v>0</v>

</xml_diff>